<commit_message>
exp 3 -- done
</commit_message>
<xml_diff>
--- a/6/3/nMOS31backup.xlsx
+++ b/6/3/nMOS31backup.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="nMOS31" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -652,21 +652,28 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.883363073716343E-2"/>
-                  <c:y val="0.39955756891550082"/>
+                  <c:x val="1.6757663713049594E-2"/>
+                  <c:y val="0.43585520956885832"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400"/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y (A) = 0.3419x (A)
+R² = 0.9992</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400"/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -2803,11 +2810,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72913408"/>
-        <c:axId val="521229952"/>
+        <c:axId val="671678464"/>
+        <c:axId val="671679040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72913408"/>
+        <c:axId val="671678464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,12 +2853,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="521229952"/>
+        <c:crossAx val="671679040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="521229952"/>
+        <c:axId val="671679040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72913408"/>
+        <c:crossAx val="671678464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>